<commit_message>
Updated BOM with Dubey PCB v2 link
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -150,7 +150,7 @@
     <t>terminal blocks 5-pack</t>
   </si>
   <si>
-    <t>https://oshpark.com/shared_projects/MSq90mky</t>
+    <t>https://oshpark.com/shared_projects/E8F8le0Q</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
General improvements to legibility (comments)
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\My Drive\projects\RPI\cubey\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BB5A83-06E7-4E3D-A445-67BF441EDAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -81,9 +87,6 @@
     <t>In addition to the above, you'll ned to 3D-print the actual robot frame.</t>
   </si>
   <si>
-    <t>I also laser-cut an acrylic sheet to form the case. That was about $40.</t>
-  </si>
-  <si>
     <t>Stepper Motor 3-pack</t>
   </si>
   <si>
@@ -151,12 +154,15 @@
   </si>
   <si>
     <t>https://oshpark.com/shared_projects/E8F8le0Q</t>
+  </si>
+  <si>
+    <t>I also laser-cut an acrylic sheet to form the case. That was about $40. Any reasonably sturdy box should do the trick.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -319,18 +325,26 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0" tableBorderDxfId="3">
-  <autoFilter ref="A1:E18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="A1:E18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Qty"/>
-    <tableColumn id="2" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" name="Link"/>
-    <tableColumn id="4" name="Unit Price" dataDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="5" name="Total*" dataDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Qty"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Link"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Unit Price" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total*" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -657,24 +671,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" customWidth="1"/>
+    <col min="2" max="2" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -691,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -709,12 +723,12 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -727,12 +741,12 @@
         <v>53.98</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -748,12 +762,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -766,12 +780,12 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -784,12 +798,12 @@
         <v>7.49</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -802,12 +816,12 @@
         <v>85.98</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -820,12 +834,12 @@
         <v>8.99</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -838,12 +852,12 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -856,15 +870,15 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="5">
         <v>13.98</v>
@@ -874,15 +888,15 @@
         <v>13.98</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
       </c>
       <c r="D12" s="5">
         <v>5.99</v>
@@ -892,7 +906,7 @@
         <v>5.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -910,15 +924,15 @@
         <v>8.9499999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1">
         <v>37.5</v>
@@ -928,15 +942,15 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="6">
         <v>6.12</v>
@@ -946,18 +960,18 @@
         <v>6.12</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
       <c r="D16" s="6">
         <v>0.33</v>
@@ -967,18 +981,18 @@
         <v>1.98</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="6">
         <v>2.95</v>
@@ -988,10 +1002,10 @@
         <v>2.95</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -1003,24 +1017,24 @@
         <v>324.17</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>